<commit_message>
Backlog and Diagramme de classe
</commit_message>
<xml_diff>
--- a/Documentation/Backlog.xlsx
+++ b/Documentation/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnatan\Documents\GitHubInterfaceProjetESP\GestionStages\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365DE4DA-8ECC-4F88-9145-8E24663FEA9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0155EB-FF3B-4847-913B-A093FE352B4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="65">
   <si>
     <t>Ordre</t>
   </si>
@@ -177,13 +177,58 @@
   </si>
   <si>
     <t>Johnatan</t>
+  </si>
+  <si>
+    <t>*Modifier selon les demandes du client</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>avant:« Il y a un filtre par rapport a l'étudiant qui consulte.», Maintenant: **</t>
+  </si>
+  <si>
+    <t>En tant que coordonateur, je veux avoir accès a une page de restriction afin de pouvoir ajouter des restrictions concernant le stage et/ou le milieu de stage</t>
+  </si>
+  <si>
+    <t>En tant que coordonateur, je veux avoir accès a une page de restriction afin de pouvoir modifier des restrictions concernant le stage et/ ou le milieu de stage</t>
+  </si>
+  <si>
+    <t>En tant que coordonateur, je veux avoir accès a une page de restriction afin de voir la liste des restrictions</t>
+  </si>
+  <si>
+    <t>on peut modifier les critères lors d'une ajout d'un milieu de stage</t>
+  </si>
+  <si>
+    <t>on peut modifier les critères lors d'une modification d'un milieu de stage</t>
+  </si>
+  <si>
+    <t>on ne peut pas modifier les critères lors d'un visionnement d'un milieu de stage</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>on peut modifier les critères lors d'une ajout d'un stage</t>
+  </si>
+  <si>
+    <t>on peut modifier les critères lors d'une modification d'un stage</t>
+  </si>
+  <si>
+    <t>on ne peut pas modifier les critères lors d'un visionnement d'un  stage</t>
+  </si>
+  <si>
+    <t>**En tant que coordonateur, je veux voir des restrictions dans le stage</t>
+  </si>
+  <si>
+    <t>**En tant que coordonateur, je veux voir des restrictions dans le milieu de stage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,8 +265,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,8 +319,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -395,6 +460,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -403,7 +531,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -438,9 +566,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -461,6 +586,35 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calcul" xfId="4" builtinId="22"/>
@@ -473,6 +627,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFC7CE"/>
       <color rgb="FFFF5050"/>
       <color rgb="FFFF7C80"/>
     </mruColors>
@@ -753,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:D30"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,13 +930,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="21">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="21">
         <v>30</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D2">
@@ -804,13 +959,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="21">
+      <c r="A4" s="20">
         <v>2</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="21">
         <v>12</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D4">
@@ -833,13 +988,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="24">
+      <c r="A6" s="23">
         <v>3</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>15</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>28</v>
       </c>
       <c r="D6">
@@ -856,13 +1011,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="24">
+      <c r="A8" s="23">
         <v>4</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="22">
         <v>15</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>37</v>
       </c>
       <c r="D8">
@@ -879,13 +1034,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="21">
+      <c r="A10" s="20">
         <v>5</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="21">
         <v>30</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D10">
@@ -911,13 +1066,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="24">
+      <c r="A13" s="23">
         <v>6</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="22">
         <v>15</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D13">
@@ -934,13 +1089,13 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="24">
+      <c r="A15" s="23">
         <v>7</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="22">
         <v>15</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D15">
@@ -957,13 +1112,13 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="21">
+      <c r="A17" s="20">
         <v>8</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="20">
         <v>8</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>24</v>
       </c>
       <c r="D17">
@@ -980,13 +1135,13 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="24">
-        <v>9</v>
-      </c>
-      <c r="B19" s="23">
+      <c r="A19" s="23">
+        <v>9</v>
+      </c>
+      <c r="B19" s="22">
         <v>11</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>39</v>
       </c>
       <c r="D19">
@@ -994,13 +1149,13 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="24">
+      <c r="A20" s="23">
         <v>10</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="22">
         <v>11</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="18" t="s">
         <v>38</v>
       </c>
       <c r="D20">
@@ -1029,19 +1184,19 @@
       <c r="D22">
         <v>2</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
@@ -1053,13 +1208,13 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="27">
+      <c r="A24" s="26">
         <v>12</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B24" s="27">
         <v>18</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="25" t="s">
         <v>3</v>
       </c>
       <c r="D24">
@@ -1076,13 +1231,13 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="29">
+      <c r="A26" s="28">
         <v>13</v>
       </c>
-      <c r="B26" s="30">
+      <c r="B26" s="29">
         <v>23</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="24" t="s">
         <v>4</v>
       </c>
       <c r="D26">
@@ -1099,13 +1254,13 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="29">
+      <c r="A28" s="28">
         <v>14</v>
       </c>
-      <c r="B28" s="30">
+      <c r="B28" s="29">
         <v>15</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D28">
@@ -1262,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1283,13 +1438,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="21">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="21">
         <v>30</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D2">
@@ -1321,13 +1476,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="21">
+      <c r="A4" s="20">
         <v>2</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="21">
         <v>12</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D4">
@@ -1362,13 +1517,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="24">
+      <c r="A6" s="23">
         <v>3</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>15</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>28</v>
       </c>
       <c r="D6">
@@ -1385,13 +1540,13 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="24">
+      <c r="A8" s="23">
         <v>4</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="22">
         <v>15</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>37</v>
       </c>
       <c r="D8">
@@ -1408,13 +1563,13 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="21">
+      <c r="A10" s="20">
         <v>5</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="21">
         <v>30</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D10">
@@ -1440,13 +1595,13 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="24">
+      <c r="A13" s="23">
         <v>6</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="22">
         <v>15</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D13">
@@ -1463,13 +1618,13 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="24">
+      <c r="A15" s="23">
         <v>7</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="22">
         <v>15</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D15">
@@ -1486,13 +1641,13 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="21">
+      <c r="A17" s="20">
         <v>8</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="20">
         <v>8</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>24</v>
       </c>
       <c r="D17">
@@ -1509,13 +1664,13 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="24">
-        <v>9</v>
-      </c>
-      <c r="B19" s="23">
+      <c r="A19" s="23">
+        <v>9</v>
+      </c>
+      <c r="B19" s="22">
         <v>11</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>39</v>
       </c>
       <c r="D19">
@@ -1523,13 +1678,13 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="24">
+      <c r="A20" s="23">
         <v>10</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="22">
         <v>11</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="18" t="s">
         <v>38</v>
       </c>
       <c r="D20">
@@ -1543,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55A5B5B-8870-4E0B-A466-F0180B642ED3}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1567,13 +1722,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="27">
+      <c r="A2" s="26">
         <v>12</v>
       </c>
-      <c r="B2" s="28">
-        <v>18</v>
-      </c>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="27">
+        <v>20</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>3</v>
       </c>
       <c r="D2">
@@ -1594,7 +1749,7 @@
       <c r="C3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="39" t="s">
         <v>18</v>
       </c>
       <c r="H3">
@@ -1605,13 +1760,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>13</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="29">
         <v>23</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="24" t="s">
         <v>4</v>
       </c>
       <c r="D4">
@@ -1646,13 +1801,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="29">
+      <c r="A6" s="28">
         <v>14</v>
       </c>
-      <c r="B6" s="30">
-        <v>15</v>
-      </c>
-      <c r="C6" s="25" t="s">
+      <c r="B6" s="29">
+        <v>5</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D6">
@@ -1661,20 +1816,182 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="8" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="41">
+        <v>19</v>
+      </c>
+      <c r="B9" s="41">
+        <v>10</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="34"/>
+      <c r="C10" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="41">
+        <v>20</v>
+      </c>
+      <c r="B11" s="41">
+        <v>10</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="34"/>
+      <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="41">
+        <v>21</v>
+      </c>
+      <c r="B13" s="41">
+        <v>5</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="38"/>
+      <c r="C14" s="44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="42">
+        <v>22</v>
+      </c>
+      <c r="B15" s="42">
+        <v>15</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8" t="s">
-        <v>13</v>
+      <c r="B17" s="43"/>
+      <c r="C17" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="43"/>
+      <c r="C18" s="37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="42">
+        <v>23</v>
+      </c>
+      <c r="B19" s="42">
+        <v>15</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="43"/>
+      <c r="C20" s="37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="43"/>
+      <c r="C21" s="37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="43"/>
+      <c r="C22" s="37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C26" s="31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="32" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de chips pour restriction
</commit_message>
<xml_diff>
--- a/Documentation/Backlog.xlsx
+++ b/Documentation/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnatan\Documents\GitHubInterfaceProjetESP\GestionStages\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4762682B-E0BD-4526-B6CB-2ACBC7ADCA53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC53724-734E-48B8-9CE2-4A21A24756B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -560,7 +560,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -637,13 +637,18 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calcul" xfId="4" builtinId="22"/>
@@ -1213,19 +1218,19 @@
       <c r="D22">
         <v>2</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="E22" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
@@ -1730,7 +1735,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1743,15 +1748,15 @@
       <c r="A1" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="43"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="45"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1765,13 +1770,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="26">
+      <c r="A5" s="20">
         <v>12</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="21">
         <v>20</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="18" t="s">
         <v>3</v>
       </c>
       <c r="D5">
@@ -1844,13 +1849,13 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="28">
+      <c r="A9" s="47">
         <v>14</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="48">
         <v>5</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="49" t="s">
         <v>40</v>
       </c>
       <c r="D9">

</xml_diff>